<commit_message>
Mise à jour Doc
</commit_message>
<xml_diff>
--- a/Documentation - Bataille Navale/Stratégie de test.xlsx
+++ b/Documentation - Bataille Navale/Stratégie de test.xlsx
@@ -147,7 +147,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -168,7 +168,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -458,7 +458,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,12 +923,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H16">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",I2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mise a jour code / doc
</commit_message>
<xml_diff>
--- a/Documentation - Bataille Navale/Stratégie de test.xlsx
+++ b/Documentation - Bataille Navale/Stratégie de test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Scénario</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Dylan Berney</t>
+  </si>
+  <si>
+    <t>Si on rentre une chiffre sup à 9 que cela fonctionne ?</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A13" sqref="A13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +682,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -698,7 +701,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -706,18 +709,18 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -736,7 +739,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -755,7 +758,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -772,15 +775,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -788,7 +802,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -796,7 +810,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -804,7 +818,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -812,7 +826,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -820,7 +834,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -828,7 +842,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -836,7 +850,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -844,7 +858,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -852,7 +866,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -860,7 +874,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -868,7 +882,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -876,7 +890,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -884,27 +898,17 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A23:F23"/>
+  <mergeCells count="31">
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A22:F22"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
@@ -916,18 +920,37 @@
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",I2)))</formula>
     </cfRule>
@@ -949,7 +972,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G2:G30</xm:sqref>
+          <xm:sqref>G2:G31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{99E24DFC-455D-476F-93D3-4666E038A2DF}">
@@ -963,7 +986,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:H16</xm:sqref>
+          <xm:sqref>H2:H17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{1A14BE9C-4481-4CE6-BCA0-599BFE2B961E}">
@@ -977,7 +1000,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I2:I16</xm:sqref>
+          <xm:sqref>I2:I17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>